<commit_message>
Update to spreadsheets etc.
</commit_message>
<xml_diff>
--- a/06_find_changes/02_change_thresholds_details/06_merge_gmw_core_tile_stats/gmw_prj_core_sar_stats.xlsx
+++ b/06_find_changes/02_change_thresholds_details/06_merge_gmw_core_tile_stats/gmw_prj_core_sar_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/Development/globalmangrovewatch/gmw_jaxa_sar_change_analysis/06_find_changes/02_change_thresholds_details/06_merge_gmw_core_tile_stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F7A0F0-00DE-C64E-B2B6-F99DC7338DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9096FEA2-4F44-D94B-ADC3-69A5C84EC752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="26460" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="26460" windowHeight="15880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hh_mean" sheetId="1" r:id="rId1"/>
@@ -957,7 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
@@ -5789,9 +5789,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
@@ -10615,9 +10621,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
@@ -15141,9 +15153,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">

</xml_diff>